<commit_message>
some changes to the prnting
</commit_message>
<xml_diff>
--- a/results/wx02/keypoints/Distance Ratio Statistics.xlsx
+++ b/results/wx02/keypoints/Distance Ratio Statistics.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" state="visible" r:id="rId2"/>
@@ -84,6 +84,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -105,6 +106,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -177,8 +179,8 @@
   </sheetPr>
   <dimension ref="A2:P30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19:P19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -186,7 +188,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.24"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.96"/>
@@ -405,7 +407,7 @@
       </c>
       <c r="D6" s="0" t="e">
         <f aca="false"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>45.1082</v>
@@ -424,7 +426,7 @@
       </c>
       <c r="J6" s="0" t="e">
         <f aca="false"/>
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
       <c r="K6" s="0" t="n">
         <v>-1.67373664415987</v>
@@ -457,7 +459,7 @@
       </c>
       <c r="D7" s="0" t="e">
         <f aca="false"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>45.1082</v>
@@ -476,7 +478,7 @@
       </c>
       <c r="J7" s="0" t="e">
         <f aca="false"/>
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
       <c r="K7" s="0" t="n">
         <v>-1.6720016569721</v>
@@ -509,7 +511,7 @@
       </c>
       <c r="D8" s="0" t="e">
         <f aca="false"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>45.1082</v>
@@ -528,7 +530,7 @@
       </c>
       <c r="J8" s="0" t="e">
         <f aca="false"/>
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
       <c r="K8" s="0" t="n">
         <v>-1.70258230865387</v>
@@ -561,7 +563,7 @@
       </c>
       <c r="D9" s="0" t="e">
         <f aca="false"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>45.648</v>
@@ -580,7 +582,7 @@
       </c>
       <c r="J9" s="0" t="e">
         <f aca="false"/>
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
       <c r="K9" s="0" t="n">
         <v>-1.7213060376604</v>
@@ -613,7 +615,7 @@
       </c>
       <c r="D10" s="0" t="e">
         <f aca="false"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>45.1082</v>
@@ -632,7 +634,7 @@
       </c>
       <c r="J10" s="0" t="e">
         <f aca="false"/>
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
       <c r="K10" s="0" t="n">
         <v>-1.69883019867945</v>
@@ -665,7 +667,7 @@
       </c>
       <c r="D11" s="0" t="e">
         <f aca="false"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>45.1082</v>
@@ -684,7 +686,7 @@
       </c>
       <c r="J11" s="0" t="e">
         <f aca="false"/>
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
       <c r="K11" s="0" t="n">
         <v>-1.69883019867945</v>
@@ -717,7 +719,7 @@
       </c>
       <c r="D12" s="0" t="e">
         <f aca="false"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>45.1082</v>
@@ -736,7 +738,7 @@
       </c>
       <c r="J12" s="0" t="e">
         <f aca="false"/>
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
       <c r="K12" s="0" t="n">
         <v>-1.70374561571673</v>
@@ -769,7 +771,7 @@
       </c>
       <c r="D13" s="0" t="e">
         <f aca="false"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>14.253</v>
@@ -920,7 +922,7 @@
       </c>
       <c r="D16" s="0" t="e">
         <f aca="false"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>14.0342</v>
@@ -1064,7 +1066,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>30.340575</v>
+        <v>3.6</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>9.29362481116088</v>
@@ -1182,8 +1184,8 @@
   </sheetPr>
   <dimension ref="A2:P30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19:P19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1191,7 +1193,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.35"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.96"/>
@@ -1410,7 +1412,7 @@
       </c>
       <c r="D6" s="0" t="e">
         <f aca="false"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>28.472855</v>
@@ -1429,11 +1431,11 @@
       </c>
       <c r="J6" s="0" t="e">
         <f aca="false"/>
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
       <c r="K6" s="0" t="e">
         <f aca="false"/>
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
       <c r="L6" s="0" t="n">
         <v>41.13709</v>
@@ -1463,7 +1465,7 @@
       </c>
       <c r="D7" s="0" t="e">
         <f aca="false"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>28.76095</v>
@@ -1482,11 +1484,11 @@
       </c>
       <c r="J7" s="0" t="e">
         <f aca="false"/>
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
       <c r="K7" s="0" t="e">
         <f aca="false"/>
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
       <c r="L7" s="0" t="n">
         <v>40.5609</v>
@@ -1516,7 +1518,7 @@
       </c>
       <c r="D8" s="0" t="e">
         <f aca="false"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>27.85851</v>
@@ -1535,11 +1537,11 @@
       </c>
       <c r="J8" s="0" t="e">
         <f aca="false"/>
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
       <c r="K8" s="0" t="e">
         <f aca="false"/>
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
       <c r="L8" s="0" t="n">
         <v>39.99878</v>
@@ -1569,7 +1571,7 @@
       </c>
       <c r="D9" s="0" t="e">
         <f aca="false"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>27.20456</v>
@@ -1588,11 +1590,11 @@
       </c>
       <c r="J9" s="0" t="e">
         <f aca="false"/>
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
       <c r="K9" s="0" t="e">
         <f aca="false"/>
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
       <c r="L9" s="0" t="n">
         <v>40.27068</v>
@@ -1622,7 +1624,7 @@
       </c>
       <c r="D10" s="0" t="e">
         <f aca="false"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>27.58336</v>
@@ -1641,11 +1643,11 @@
       </c>
       <c r="J10" s="0" t="e">
         <f aca="false"/>
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
       <c r="K10" s="0" t="e">
         <f aca="false"/>
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
       <c r="L10" s="0" t="n">
         <v>41.02828</v>
@@ -1675,7 +1677,7 @@
       </c>
       <c r="D11" s="0" t="e">
         <f aca="false"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>27.58336</v>
@@ -1694,11 +1696,11 @@
       </c>
       <c r="J11" s="0" t="e">
         <f aca="false"/>
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
       <c r="K11" s="0" t="e">
         <f aca="false"/>
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
       <c r="L11" s="0" t="n">
         <v>41.02828</v>
@@ -1728,7 +1730,7 @@
       </c>
       <c r="D12" s="0" t="e">
         <f aca="false"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>27.46356</v>
@@ -1747,11 +1749,11 @@
       </c>
       <c r="J12" s="0" t="e">
         <f aca="false"/>
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
       <c r="K12" s="0" t="e">
         <f aca="false"/>
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
       <c r="L12" s="0" t="n">
         <v>40.78868</v>
@@ -1781,7 +1783,7 @@
       </c>
       <c r="D13" s="0" t="e">
         <f aca="false"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>11.727875</v>
@@ -1932,7 +1934,7 @@
       </c>
       <c r="D16" s="0" t="e">
         <f aca="false"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>13.8154</v>
@@ -2051,7 +2053,7 @@
       </c>
       <c r="J18" s="0" t="e">
         <f aca="false"/>
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
       <c r="K18" s="0" t="n">
         <v>1.73205080756888</v>
@@ -2102,7 +2104,7 @@
       </c>
       <c r="J19" s="0" t="e">
         <f aca="false"/>
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
       <c r="K19" s="0" t="n">
         <v>1.73205080756888</v>
@@ -2181,7 +2183,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2197,7 +2199,7 @@
   <dimension ref="A2:P30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K36" activeCellId="1" sqref="B19:P19 K36"/>
+      <selection pane="topLeft" activeCell="K36" activeCellId="0" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2205,7 +2207,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.35"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.96"/>
@@ -2471,7 +2473,7 @@
       </c>
       <c r="D6" s="0" t="e">
         <f aca="false">'Without Outliers'!D6/All!D6</f>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="E6" s="0" t="n">
         <f aca="false">'Without Outliers'!E6/All!E6</f>
@@ -2495,11 +2497,11 @@
       </c>
       <c r="J6" s="0" t="e">
         <f aca="false">'Without Outliers'!J6/All!J6</f>
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
       <c r="K6" s="0" t="e">
         <f aca="false">'Without Outliers'!K6/All!K6</f>
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
       <c r="L6" s="0" t="n">
         <f aca="false">'Without Outliers'!L6/All!L6</f>
@@ -2536,7 +2538,7 @@
       </c>
       <c r="D7" s="0" t="e">
         <f aca="false">'Without Outliers'!D7/All!D7</f>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="E7" s="0" t="n">
         <f aca="false">'Without Outliers'!E7/All!E7</f>
@@ -2560,11 +2562,11 @@
       </c>
       <c r="J7" s="0" t="e">
         <f aca="false">'Without Outliers'!J7/All!J7</f>
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
       <c r="K7" s="0" t="e">
         <f aca="false">'Without Outliers'!K7/All!K7</f>
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
       <c r="L7" s="0" t="n">
         <f aca="false">'Without Outliers'!L7/All!L7</f>
@@ -2601,7 +2603,7 @@
       </c>
       <c r="D8" s="0" t="e">
         <f aca="false">'Without Outliers'!D8/All!D8</f>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="E8" s="0" t="n">
         <f aca="false">'Without Outliers'!E8/All!E8</f>
@@ -2625,11 +2627,11 @@
       </c>
       <c r="J8" s="0" t="e">
         <f aca="false">'Without Outliers'!J8/All!J8</f>
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
       <c r="K8" s="0" t="e">
         <f aca="false">'Without Outliers'!K8/All!K8</f>
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
       <c r="L8" s="0" t="n">
         <f aca="false">'Without Outliers'!L8/All!L8</f>
@@ -2666,7 +2668,7 @@
       </c>
       <c r="D9" s="0" t="e">
         <f aca="false">'Without Outliers'!D9/All!D9</f>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="E9" s="0" t="n">
         <f aca="false">'Without Outliers'!E9/All!E9</f>
@@ -2690,11 +2692,11 @@
       </c>
       <c r="J9" s="0" t="e">
         <f aca="false">'Without Outliers'!J9/All!J9</f>
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
       <c r="K9" s="0" t="e">
         <f aca="false">'Without Outliers'!K9/All!K9</f>
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
       <c r="L9" s="0" t="n">
         <f aca="false">'Without Outliers'!L9/All!L9</f>
@@ -2731,7 +2733,7 @@
       </c>
       <c r="D10" s="0" t="e">
         <f aca="false">'Without Outliers'!D10/All!D10</f>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="E10" s="0" t="n">
         <f aca="false">'Without Outliers'!E10/All!E10</f>
@@ -2755,11 +2757,11 @@
       </c>
       <c r="J10" s="0" t="e">
         <f aca="false">'Without Outliers'!J10/All!J10</f>
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
       <c r="K10" s="0" t="e">
         <f aca="false">'Without Outliers'!K10/All!K10</f>
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
       <c r="L10" s="0" t="n">
         <f aca="false">'Without Outliers'!L10/All!L10</f>
@@ -2796,7 +2798,7 @@
       </c>
       <c r="D11" s="0" t="e">
         <f aca="false">'Without Outliers'!D11/All!D11</f>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="E11" s="0" t="n">
         <f aca="false">'Without Outliers'!E11/All!E11</f>
@@ -2820,11 +2822,11 @@
       </c>
       <c r="J11" s="0" t="e">
         <f aca="false">'Without Outliers'!J11/All!J11</f>
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
       <c r="K11" s="0" t="e">
         <f aca="false">'Without Outliers'!K11/All!K11</f>
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
       <c r="L11" s="0" t="n">
         <f aca="false">'Without Outliers'!L11/All!L11</f>
@@ -2861,7 +2863,7 @@
       </c>
       <c r="D12" s="0" t="e">
         <f aca="false">'Without Outliers'!D12/All!D12</f>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="E12" s="0" t="n">
         <f aca="false">'Without Outliers'!E12/All!E12</f>
@@ -2885,11 +2887,11 @@
       </c>
       <c r="J12" s="0" t="e">
         <f aca="false">'Without Outliers'!J12/All!J12</f>
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
       <c r="K12" s="0" t="e">
         <f aca="false">'Without Outliers'!K12/All!K12</f>
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
       <c r="L12" s="0" t="n">
         <f aca="false">'Without Outliers'!L12/All!L12</f>
@@ -2926,7 +2928,7 @@
       </c>
       <c r="D13" s="0" t="e">
         <f aca="false">'Without Outliers'!D13/All!D13</f>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="E13" s="0" t="n">
         <f aca="false">'Without Outliers'!E13/All!E13</f>
@@ -3121,7 +3123,7 @@
       </c>
       <c r="D16" s="0" t="e">
         <f aca="false">'Without Outliers'!D16/All!D16</f>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="E16" s="0" t="n">
         <f aca="false">'Without Outliers'!E16/All!E16</f>
@@ -3275,7 +3277,7 @@
       </c>
       <c r="J18" s="0" t="e">
         <f aca="false">'Without Outliers'!J18/All!J18</f>
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
       <c r="K18" s="0" t="n">
         <f aca="false">'Without Outliers'!K18/All!K18</f>
@@ -3308,7 +3310,7 @@
       </c>
       <c r="B19" s="0" t="n">
         <f aca="false">'Without Outliers'!B19/All!B19</f>
-        <v>0.814684626115359</v>
+        <v>6.86611111111111</v>
       </c>
       <c r="C19" s="0" t="n">
         <f aca="false">'Without Outliers'!C19/All!C19</f>
@@ -3340,7 +3342,7 @@
       </c>
       <c r="J19" s="0" t="e">
         <f aca="false">'Without Outliers'!J19/All!J19</f>
-        <v>#NUM!</v>
+        <v>#N/A</v>
       </c>
       <c r="K19" s="0" t="n">
         <f aca="false">'Without Outliers'!K19/All!K19</f>
@@ -4085,7 +4087,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>